<commit_message>
minor changes in naming convention
</commit_message>
<xml_diff>
--- a/Resources/TestData.xlsx
+++ b/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/hrithik_neogi_capgemini_com/Documents/Documents/L1 Training/Sprint2/payback-explore/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC1048AA59D849E05ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD535423-B1F7-4C95-B79D-E22D4C7319F2}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC1048AA59D849E05ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8E43107-7823-4127-AA34-04E9CD54503E}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3860" yWindow="2630" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
     <t>Know About Payback</t>
   </si>
   <si>
-    <t>https://www.payback.in/</t>
+    <t>https://www.payback.in/offers</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>